<commit_message>
added beginning part of pseudo code to median income notebook
</commit_message>
<xml_diff>
--- a/Resources/State_Median_Income.xlsx
+++ b/Resources/State_Median_Income.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvolo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvolo\dumbledores_platoon\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{611B18E2-E7C6-45AB-94FC-DADA8A148611}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C49AB090-0BC3-4B8E-9B78-75CF8E3E1ED9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -388,7 +388,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -441,11 +441,100 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFAAC1D9"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFAAC1D9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFAAC1D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFAAC1D9"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFAAC1D9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFAAC1D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFAAC1D9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFAAC1D9"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFAAC1D9"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFAAC1D9"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFAAC1D9"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FFAAC1D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFFFFFF"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FFAAC1D9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFAAC1D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFAAC1D9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFAAC1D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFAAC1D9"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFAAC1D9"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -456,19 +545,40 @@
     <xf numFmtId="3" fontId="6" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -811,7 +921,7 @@
   <dimension ref="A1:BY115"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:BY1"/>
+      <selection activeCell="G64" sqref="G64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -821,488 +931,488 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:77" ht="3" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
-      <c r="P1" s="4"/>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-      <c r="T1" s="4"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="4"/>
-      <c r="Y1" s="4"/>
-      <c r="Z1" s="4"/>
-      <c r="AA1" s="4"/>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4"/>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
-      <c r="AJ1" s="4"/>
-      <c r="AK1" s="4"/>
-      <c r="AL1" s="4"/>
-      <c r="AM1" s="4"/>
-      <c r="AN1" s="4"/>
-      <c r="AO1" s="4"/>
-      <c r="AP1" s="4"/>
-      <c r="AQ1" s="4"/>
-      <c r="AR1" s="4"/>
-      <c r="AS1" s="4"/>
-      <c r="AT1" s="4"/>
-      <c r="AU1" s="4"/>
-      <c r="AV1" s="4"/>
-      <c r="AW1" s="4"/>
-      <c r="AX1" s="4"/>
-      <c r="AY1" s="4"/>
-      <c r="AZ1" s="4"/>
-      <c r="BA1" s="4"/>
-      <c r="BB1" s="4"/>
-      <c r="BC1" s="4"/>
-      <c r="BD1" s="4"/>
-      <c r="BE1" s="4"/>
-      <c r="BF1" s="4"/>
-      <c r="BG1" s="4"/>
-      <c r="BH1" s="4"/>
-      <c r="BI1" s="4"/>
-      <c r="BJ1" s="4"/>
-      <c r="BK1" s="4"/>
-      <c r="BL1" s="4"/>
-      <c r="BM1" s="4"/>
-      <c r="BN1" s="4"/>
-      <c r="BO1" s="4"/>
-      <c r="BP1" s="4"/>
-      <c r="BQ1" s="4"/>
-      <c r="BR1" s="4"/>
-      <c r="BS1" s="4"/>
-      <c r="BT1" s="4"/>
-      <c r="BU1" s="4"/>
-      <c r="BV1" s="4"/>
-      <c r="BW1" s="4"/>
-      <c r="BX1" s="4"/>
-      <c r="BY1" s="4"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="7"/>
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="7"/>
+      <c r="N1" s="7"/>
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+      <c r="AA1" s="7"/>
+      <c r="AB1" s="7"/>
+      <c r="AC1" s="7"/>
+      <c r="AD1" s="7"/>
+      <c r="AE1" s="7"/>
+      <c r="AF1" s="7"/>
+      <c r="AG1" s="7"/>
+      <c r="AH1" s="7"/>
+      <c r="AI1" s="7"/>
+      <c r="AJ1" s="7"/>
+      <c r="AK1" s="7"/>
+      <c r="AL1" s="7"/>
+      <c r="AM1" s="7"/>
+      <c r="AN1" s="7"/>
+      <c r="AO1" s="7"/>
+      <c r="AP1" s="7"/>
+      <c r="AQ1" s="7"/>
+      <c r="AR1" s="7"/>
+      <c r="AS1" s="7"/>
+      <c r="AT1" s="7"/>
+      <c r="AU1" s="7"/>
+      <c r="AV1" s="7"/>
+      <c r="AW1" s="7"/>
+      <c r="AX1" s="7"/>
+      <c r="AY1" s="7"/>
+      <c r="AZ1" s="7"/>
+      <c r="BA1" s="7"/>
+      <c r="BB1" s="7"/>
+      <c r="BC1" s="7"/>
+      <c r="BD1" s="7"/>
+      <c r="BE1" s="7"/>
+      <c r="BF1" s="7"/>
+      <c r="BG1" s="7"/>
+      <c r="BH1" s="7"/>
+      <c r="BI1" s="7"/>
+      <c r="BJ1" s="7"/>
+      <c r="BK1" s="7"/>
+      <c r="BL1" s="7"/>
+      <c r="BM1" s="7"/>
+      <c r="BN1" s="7"/>
+      <c r="BO1" s="7"/>
+      <c r="BP1" s="7"/>
+      <c r="BQ1" s="7"/>
+      <c r="BR1" s="7"/>
+      <c r="BS1" s="7"/>
+      <c r="BT1" s="7"/>
+      <c r="BU1" s="7"/>
+      <c r="BV1" s="7"/>
+      <c r="BW1" s="7"/>
+      <c r="BX1" s="7"/>
+      <c r="BY1" s="7"/>
     </row>
     <row r="2" spans="1:77" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="5"/>
-      <c r="W2" s="5"/>
-      <c r="X2" s="5"/>
-      <c r="Y2" s="5"/>
-      <c r="Z2" s="5"/>
-      <c r="AA2" s="5"/>
-      <c r="AB2" s="5"/>
-      <c r="AC2" s="5"/>
-      <c r="AD2" s="5"/>
-      <c r="AE2" s="5"/>
-      <c r="AF2" s="5"/>
-      <c r="AG2" s="5"/>
-      <c r="AH2" s="5"/>
-      <c r="AI2" s="5"/>
-      <c r="AJ2" s="5"/>
-      <c r="AK2" s="5"/>
-      <c r="AL2" s="5"/>
-      <c r="AM2" s="5"/>
-      <c r="AN2" s="5"/>
-      <c r="AO2" s="5"/>
-      <c r="AP2" s="5"/>
-      <c r="AQ2" s="5"/>
-      <c r="AR2" s="5"/>
-      <c r="AS2" s="5"/>
-      <c r="AT2" s="5"/>
-      <c r="AU2" s="5"/>
-      <c r="AV2" s="5"/>
-      <c r="AW2" s="5"/>
-      <c r="AX2" s="5"/>
-      <c r="AY2" s="5"/>
-      <c r="AZ2" s="5"/>
-      <c r="BA2" s="5"/>
-      <c r="BB2" s="5"/>
-      <c r="BC2" s="5"/>
-      <c r="BD2" s="5"/>
-      <c r="BE2" s="5"/>
-      <c r="BF2" s="5"/>
-      <c r="BG2" s="5"/>
-      <c r="BH2" s="5"/>
-      <c r="BI2" s="5"/>
-      <c r="BJ2" s="5"/>
-      <c r="BK2" s="5"/>
-      <c r="BL2" s="5"/>
-      <c r="BM2" s="5"/>
-      <c r="BN2" s="5"/>
-      <c r="BO2" s="5"/>
-      <c r="BP2" s="5"/>
-      <c r="BQ2" s="5"/>
-      <c r="BR2" s="5"/>
-      <c r="BS2" s="5"/>
-      <c r="BT2" s="5"/>
-      <c r="BU2" s="5"/>
-      <c r="BV2" s="5"/>
-      <c r="BW2" s="5"/>
-      <c r="BX2" s="5"/>
-      <c r="BY2" s="5"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="8"/>
+      <c r="R2" s="8"/>
+      <c r="S2" s="8"/>
+      <c r="T2" s="8"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
+      <c r="X2" s="8"/>
+      <c r="Y2" s="8"/>
+      <c r="Z2" s="8"/>
+      <c r="AA2" s="8"/>
+      <c r="AB2" s="8"/>
+      <c r="AC2" s="8"/>
+      <c r="AD2" s="8"/>
+      <c r="AE2" s="8"/>
+      <c r="AF2" s="8"/>
+      <c r="AG2" s="8"/>
+      <c r="AH2" s="8"/>
+      <c r="AI2" s="8"/>
+      <c r="AJ2" s="8"/>
+      <c r="AK2" s="8"/>
+      <c r="AL2" s="8"/>
+      <c r="AM2" s="8"/>
+      <c r="AN2" s="8"/>
+      <c r="AO2" s="8"/>
+      <c r="AP2" s="8"/>
+      <c r="AQ2" s="8"/>
+      <c r="AR2" s="8"/>
+      <c r="AS2" s="8"/>
+      <c r="AT2" s="8"/>
+      <c r="AU2" s="8"/>
+      <c r="AV2" s="8"/>
+      <c r="AW2" s="8"/>
+      <c r="AX2" s="8"/>
+      <c r="AY2" s="8"/>
+      <c r="AZ2" s="8"/>
+      <c r="BA2" s="8"/>
+      <c r="BB2" s="8"/>
+      <c r="BC2" s="8"/>
+      <c r="BD2" s="8"/>
+      <c r="BE2" s="8"/>
+      <c r="BF2" s="8"/>
+      <c r="BG2" s="8"/>
+      <c r="BH2" s="8"/>
+      <c r="BI2" s="8"/>
+      <c r="BJ2" s="8"/>
+      <c r="BK2" s="8"/>
+      <c r="BL2" s="8"/>
+      <c r="BM2" s="8"/>
+      <c r="BN2" s="8"/>
+      <c r="BO2" s="8"/>
+      <c r="BP2" s="8"/>
+      <c r="BQ2" s="8"/>
+      <c r="BR2" s="8"/>
+      <c r="BS2" s="8"/>
+      <c r="BT2" s="8"/>
+      <c r="BU2" s="8"/>
+      <c r="BV2" s="8"/>
+      <c r="BW2" s="8"/>
+      <c r="BX2" s="8"/>
+      <c r="BY2" s="8"/>
     </row>
     <row r="3" spans="1:77" x14ac:dyDescent="0.3">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="6"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="6"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="6"/>
-      <c r="AH3" s="6"/>
-      <c r="AI3" s="6"/>
-      <c r="AJ3" s="6"/>
-      <c r="AK3" s="6"/>
-      <c r="AL3" s="6"/>
-      <c r="AM3" s="6"/>
-      <c r="AN3" s="6"/>
-      <c r="AO3" s="6"/>
-      <c r="AP3" s="6"/>
-      <c r="AQ3" s="6"/>
-      <c r="AR3" s="6"/>
-      <c r="AS3" s="6"/>
-      <c r="AT3" s="6"/>
-      <c r="AU3" s="6"/>
-      <c r="AV3" s="6"/>
-      <c r="AW3" s="6"/>
-      <c r="AX3" s="6"/>
-      <c r="AY3" s="6"/>
-      <c r="AZ3" s="6"/>
-      <c r="BA3" s="6"/>
-      <c r="BB3" s="6"/>
-      <c r="BC3" s="6"/>
-      <c r="BD3" s="6"/>
-      <c r="BE3" s="6"/>
-      <c r="BF3" s="6"/>
-      <c r="BG3" s="6"/>
-      <c r="BH3" s="6"/>
-      <c r="BI3" s="6"/>
-      <c r="BJ3" s="6"/>
-      <c r="BK3" s="6"/>
-      <c r="BL3" s="6"/>
-      <c r="BM3" s="6"/>
-      <c r="BN3" s="6"/>
-      <c r="BO3" s="6"/>
-      <c r="BP3" s="6"/>
-      <c r="BQ3" s="6"/>
-      <c r="BR3" s="6"/>
-      <c r="BS3" s="6"/>
-      <c r="BT3" s="6"/>
-      <c r="BU3" s="6"/>
-      <c r="BV3" s="6"/>
-      <c r="BW3" s="6"/>
-      <c r="BX3" s="6"/>
-      <c r="BY3" s="6"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="9"/>
+      <c r="J3" s="9"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="9"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="9"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="9"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="9"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="9"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="9"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="9"/>
+      <c r="AG3" s="9"/>
+      <c r="AH3" s="9"/>
+      <c r="AI3" s="9"/>
+      <c r="AJ3" s="9"/>
+      <c r="AK3" s="9"/>
+      <c r="AL3" s="9"/>
+      <c r="AM3" s="9"/>
+      <c r="AN3" s="9"/>
+      <c r="AO3" s="9"/>
+      <c r="AP3" s="9"/>
+      <c r="AQ3" s="9"/>
+      <c r="AR3" s="9"/>
+      <c r="AS3" s="9"/>
+      <c r="AT3" s="9"/>
+      <c r="AU3" s="9"/>
+      <c r="AV3" s="9"/>
+      <c r="AW3" s="9"/>
+      <c r="AX3" s="9"/>
+      <c r="AY3" s="9"/>
+      <c r="AZ3" s="9"/>
+      <c r="BA3" s="9"/>
+      <c r="BB3" s="9"/>
+      <c r="BC3" s="9"/>
+      <c r="BD3" s="9"/>
+      <c r="BE3" s="9"/>
+      <c r="BF3" s="9"/>
+      <c r="BG3" s="9"/>
+      <c r="BH3" s="9"/>
+      <c r="BI3" s="9"/>
+      <c r="BJ3" s="9"/>
+      <c r="BK3" s="9"/>
+      <c r="BL3" s="9"/>
+      <c r="BM3" s="9"/>
+      <c r="BN3" s="9"/>
+      <c r="BO3" s="9"/>
+      <c r="BP3" s="9"/>
+      <c r="BQ3" s="9"/>
+      <c r="BR3" s="9"/>
+      <c r="BS3" s="9"/>
+      <c r="BT3" s="9"/>
+      <c r="BU3" s="9"/>
+      <c r="BV3" s="9"/>
+      <c r="BW3" s="9"/>
+      <c r="BX3" s="9"/>
+      <c r="BY3" s="9"/>
     </row>
     <row r="4" spans="1:77" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+      <c r="A4" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="7"/>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
-      <c r="I4" s="7"/>
-      <c r="J4" s="7"/>
-      <c r="K4" s="7"/>
-      <c r="L4" s="7"/>
-      <c r="M4" s="7"/>
-      <c r="N4" s="7"/>
-      <c r="O4" s="7"/>
-      <c r="P4" s="7"/>
-      <c r="Q4" s="7"/>
-      <c r="R4" s="7"/>
-      <c r="S4" s="7"/>
-      <c r="T4" s="7"/>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="7"/>
-      <c r="AD4" s="7"/>
-      <c r="AE4" s="7"/>
-      <c r="AF4" s="7"/>
-      <c r="AG4" s="7"/>
-      <c r="AH4" s="7"/>
-      <c r="AI4" s="7"/>
-      <c r="AJ4" s="7"/>
-      <c r="AK4" s="7"/>
-      <c r="AL4" s="7"/>
-      <c r="AM4" s="7"/>
-      <c r="AN4" s="7"/>
-      <c r="AO4" s="7"/>
-      <c r="AP4" s="7"/>
-      <c r="AQ4" s="7"/>
-      <c r="AR4" s="7"/>
-      <c r="AS4" s="7"/>
-      <c r="AT4" s="7"/>
-      <c r="AU4" s="7"/>
-      <c r="AV4" s="7"/>
-      <c r="AW4" s="7"/>
-      <c r="AX4" s="7"/>
-      <c r="AY4" s="7"/>
-      <c r="AZ4" s="7"/>
-      <c r="BA4" s="7"/>
-      <c r="BB4" s="7"/>
-      <c r="BC4" s="7"/>
-      <c r="BD4" s="7"/>
-      <c r="BE4" s="7"/>
-      <c r="BF4" s="7"/>
-      <c r="BG4" s="7"/>
-      <c r="BH4" s="7"/>
-      <c r="BI4" s="7"/>
-      <c r="BJ4" s="7"/>
-      <c r="BK4" s="7"/>
-      <c r="BL4" s="7"/>
-      <c r="BM4" s="7"/>
-      <c r="BN4" s="7"/>
-      <c r="BO4" s="7"/>
-      <c r="BP4" s="7"/>
-      <c r="BQ4" s="7"/>
-      <c r="BR4" s="7"/>
-      <c r="BS4" s="7"/>
-      <c r="BT4" s="7"/>
-      <c r="BU4" s="7"/>
-      <c r="BV4" s="7"/>
-      <c r="BW4" s="7"/>
-      <c r="BX4" s="7"/>
-      <c r="BY4" s="7"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="6"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="6"/>
+      <c r="AL4" s="6"/>
+      <c r="AM4" s="6"/>
+      <c r="AN4" s="6"/>
+      <c r="AO4" s="6"/>
+      <c r="AP4" s="6"/>
+      <c r="AQ4" s="6"/>
+      <c r="AR4" s="6"/>
+      <c r="AS4" s="6"/>
+      <c r="AT4" s="6"/>
+      <c r="AU4" s="6"/>
+      <c r="AV4" s="6"/>
+      <c r="AW4" s="6"/>
+      <c r="AX4" s="6"/>
+      <c r="AY4" s="6"/>
+      <c r="AZ4" s="6"/>
+      <c r="BA4" s="6"/>
+      <c r="BB4" s="6"/>
+      <c r="BC4" s="6"/>
+      <c r="BD4" s="6"/>
+      <c r="BE4" s="6"/>
+      <c r="BF4" s="6"/>
+      <c r="BG4" s="6"/>
+      <c r="BH4" s="6"/>
+      <c r="BI4" s="6"/>
+      <c r="BJ4" s="6"/>
+      <c r="BK4" s="6"/>
+      <c r="BL4" s="6"/>
+      <c r="BM4" s="6"/>
+      <c r="BN4" s="6"/>
+      <c r="BO4" s="6"/>
+      <c r="BP4" s="6"/>
+      <c r="BQ4" s="6"/>
+      <c r="BR4" s="6"/>
+      <c r="BS4" s="6"/>
+      <c r="BT4" s="6"/>
+      <c r="BU4" s="6"/>
+      <c r="BV4" s="6"/>
+      <c r="BW4" s="6"/>
+      <c r="BX4" s="6"/>
+      <c r="BY4" s="6"/>
     </row>
     <row r="5" spans="1:77" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="4">
         <v>2019</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="8">
+      <c r="C5" s="4"/>
+      <c r="D5" s="4">
         <v>2018</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8" t="s">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8">
+      <c r="G5" s="4"/>
+      <c r="H5" s="4">
         <v>2017</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8">
+      <c r="I5" s="4"/>
+      <c r="J5" s="4">
         <v>2016</v>
       </c>
-      <c r="K5" s="8"/>
-      <c r="L5" s="8">
+      <c r="K5" s="4"/>
+      <c r="L5" s="4">
         <v>2015</v>
       </c>
-      <c r="M5" s="8"/>
-      <c r="N5" s="8">
+      <c r="M5" s="4"/>
+      <c r="N5" s="4">
         <v>2014</v>
       </c>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8" t="s">
+      <c r="O5" s="4"/>
+      <c r="P5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="Q5" s="8"/>
-      <c r="R5" s="8" t="s">
+      <c r="Q5" s="4"/>
+      <c r="R5" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="S5" s="8"/>
-      <c r="T5" s="8">
+      <c r="S5" s="4"/>
+      <c r="T5" s="4">
         <v>2012</v>
       </c>
-      <c r="U5" s="8"/>
-      <c r="V5" s="8">
+      <c r="U5" s="4"/>
+      <c r="V5" s="4">
         <v>2011</v>
       </c>
-      <c r="W5" s="8"/>
-      <c r="X5" s="8" t="s">
+      <c r="W5" s="4"/>
+      <c r="X5" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="Y5" s="8"/>
-      <c r="Z5" s="8" t="s">
+      <c r="Y5" s="4"/>
+      <c r="Z5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="AA5" s="8"/>
-      <c r="AB5" s="8">
+      <c r="AA5" s="4"/>
+      <c r="AB5" s="4">
         <v>2008</v>
       </c>
-      <c r="AC5" s="8"/>
-      <c r="AD5" s="8">
+      <c r="AC5" s="4"/>
+      <c r="AD5" s="4">
         <v>2007</v>
       </c>
-      <c r="AE5" s="8"/>
-      <c r="AF5" s="8">
+      <c r="AE5" s="4"/>
+      <c r="AF5" s="4">
         <v>2006</v>
       </c>
-      <c r="AG5" s="8"/>
-      <c r="AH5" s="8">
+      <c r="AG5" s="4"/>
+      <c r="AH5" s="4">
         <v>2005</v>
       </c>
-      <c r="AI5" s="8"/>
-      <c r="AJ5" s="8" t="s">
+      <c r="AI5" s="4"/>
+      <c r="AJ5" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="AK5" s="8"/>
-      <c r="AL5" s="8">
+      <c r="AK5" s="4"/>
+      <c r="AL5" s="4">
         <v>2003</v>
       </c>
-      <c r="AM5" s="8"/>
-      <c r="AN5" s="8">
+      <c r="AM5" s="4"/>
+      <c r="AN5" s="4">
         <v>2002</v>
       </c>
-      <c r="AO5" s="8"/>
-      <c r="AP5" s="8">
+      <c r="AO5" s="4"/>
+      <c r="AP5" s="4">
         <v>2001</v>
       </c>
-      <c r="AQ5" s="8"/>
-      <c r="AR5" s="8" t="s">
+      <c r="AQ5" s="4"/>
+      <c r="AR5" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="AS5" s="8"/>
-      <c r="AT5" s="8" t="s">
+      <c r="AS5" s="4"/>
+      <c r="AT5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="AU5" s="8"/>
-      <c r="AV5" s="8">
+      <c r="AU5" s="4"/>
+      <c r="AV5" s="4">
         <v>1998</v>
       </c>
-      <c r="AW5" s="8"/>
-      <c r="AX5" s="8">
+      <c r="AW5" s="4"/>
+      <c r="AX5" s="4">
         <v>1997</v>
       </c>
-      <c r="AY5" s="8"/>
-      <c r="AZ5" s="8">
+      <c r="AY5" s="4"/>
+      <c r="AZ5" s="4">
         <v>1996</v>
       </c>
-      <c r="BA5" s="8"/>
-      <c r="BB5" s="8" t="s">
+      <c r="BA5" s="4"/>
+      <c r="BB5" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="BC5" s="8"/>
-      <c r="BD5" s="8" t="s">
+      <c r="BC5" s="4"/>
+      <c r="BD5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="BE5" s="8"/>
-      <c r="BF5" s="8" t="s">
+      <c r="BE5" s="4"/>
+      <c r="BF5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="BG5" s="8"/>
-      <c r="BH5" s="8" t="s">
+      <c r="BG5" s="4"/>
+      <c r="BH5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="BI5" s="8"/>
-      <c r="BJ5" s="8">
+      <c r="BI5" s="4"/>
+      <c r="BJ5" s="4">
         <v>1991</v>
       </c>
-      <c r="BK5" s="8"/>
-      <c r="BL5" s="8">
+      <c r="BK5" s="4"/>
+      <c r="BL5" s="4">
         <v>1990</v>
       </c>
-      <c r="BM5" s="8"/>
-      <c r="BN5" s="8">
+      <c r="BM5" s="4"/>
+      <c r="BN5" s="4">
         <v>1989</v>
       </c>
-      <c r="BO5" s="8"/>
-      <c r="BP5" s="8">
+      <c r="BO5" s="4"/>
+      <c r="BP5" s="4">
         <v>1988</v>
       </c>
-      <c r="BQ5" s="8"/>
-      <c r="BR5" s="8" t="s">
+      <c r="BQ5" s="4"/>
+      <c r="BR5" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="BS5" s="8"/>
-      <c r="BT5" s="8">
+      <c r="BS5" s="4"/>
+      <c r="BT5" s="4">
         <v>1986</v>
       </c>
-      <c r="BU5" s="8"/>
-      <c r="BV5" s="8" t="s">
+      <c r="BU5" s="4"/>
+      <c r="BV5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="BW5" s="8"/>
-      <c r="BX5" s="8" t="s">
+      <c r="BW5" s="4"/>
+      <c r="BX5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="BY5" s="8"/>
+      <c r="BY5" s="4"/>
     </row>
     <row r="6" spans="1:77" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
+      <c r="A6" s="4"/>
       <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
@@ -13649,245 +13759,245 @@
       </c>
     </row>
     <row r="59" spans="1:77" x14ac:dyDescent="0.3">
-      <c r="A59" s="7" t="s">
+      <c r="A59" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B59" s="7"/>
-      <c r="C59" s="7"/>
-      <c r="D59" s="7"/>
-      <c r="E59" s="7"/>
-      <c r="F59" s="7"/>
-      <c r="G59" s="7"/>
-      <c r="H59" s="7"/>
-      <c r="I59" s="7"/>
-      <c r="J59" s="7"/>
-      <c r="K59" s="7"/>
-      <c r="L59" s="7"/>
-      <c r="M59" s="7"/>
-      <c r="N59" s="7"/>
-      <c r="O59" s="7"/>
-      <c r="P59" s="7"/>
-      <c r="Q59" s="7"/>
-      <c r="R59" s="7"/>
-      <c r="S59" s="7"/>
-      <c r="T59" s="7"/>
-      <c r="U59" s="7"/>
-      <c r="V59" s="7"/>
-      <c r="W59" s="7"/>
-      <c r="X59" s="7"/>
-      <c r="Y59" s="7"/>
-      <c r="Z59" s="7"/>
-      <c r="AA59" s="7"/>
-      <c r="AB59" s="7"/>
-      <c r="AC59" s="7"/>
-      <c r="AD59" s="7"/>
-      <c r="AE59" s="7"/>
-      <c r="AF59" s="7"/>
-      <c r="AG59" s="7"/>
-      <c r="AH59" s="7"/>
-      <c r="AI59" s="7"/>
-      <c r="AJ59" s="7"/>
-      <c r="AK59" s="7"/>
-      <c r="AL59" s="7"/>
-      <c r="AM59" s="7"/>
-      <c r="AN59" s="7"/>
-      <c r="AO59" s="7"/>
-      <c r="AP59" s="7"/>
-      <c r="AQ59" s="7"/>
-      <c r="AR59" s="7"/>
-      <c r="AS59" s="7"/>
-      <c r="AT59" s="7"/>
-      <c r="AU59" s="7"/>
-      <c r="AV59" s="7"/>
-      <c r="AW59" s="7"/>
-      <c r="AX59" s="7"/>
-      <c r="AY59" s="7"/>
-      <c r="AZ59" s="7"/>
-      <c r="BA59" s="7"/>
-      <c r="BB59" s="7"/>
-      <c r="BC59" s="7"/>
-      <c r="BD59" s="7"/>
-      <c r="BE59" s="7"/>
-      <c r="BF59" s="7"/>
-      <c r="BG59" s="7"/>
-      <c r="BH59" s="7"/>
-      <c r="BI59" s="7"/>
-      <c r="BJ59" s="7"/>
-      <c r="BK59" s="7"/>
-      <c r="BL59" s="7"/>
-      <c r="BM59" s="7"/>
-      <c r="BN59" s="7"/>
-      <c r="BO59" s="7"/>
-      <c r="BP59" s="7"/>
-      <c r="BQ59" s="7"/>
-      <c r="BR59" s="7"/>
-      <c r="BS59" s="7"/>
-      <c r="BT59" s="7"/>
-      <c r="BU59" s="7"/>
-      <c r="BV59" s="7"/>
-      <c r="BW59" s="7"/>
-      <c r="BX59" s="7"/>
-      <c r="BY59" s="7"/>
+      <c r="B59" s="15"/>
+      <c r="C59" s="15"/>
+      <c r="D59" s="15"/>
+      <c r="E59" s="15"/>
+      <c r="F59" s="15"/>
+      <c r="G59" s="15"/>
+      <c r="H59" s="15"/>
+      <c r="I59" s="15"/>
+      <c r="J59" s="15"/>
+      <c r="K59" s="15"/>
+      <c r="L59" s="15"/>
+      <c r="M59" s="15"/>
+      <c r="N59" s="15"/>
+      <c r="O59" s="15"/>
+      <c r="P59" s="15"/>
+      <c r="Q59" s="15"/>
+      <c r="R59" s="15"/>
+      <c r="S59" s="15"/>
+      <c r="T59" s="15"/>
+      <c r="U59" s="15"/>
+      <c r="V59" s="15"/>
+      <c r="W59" s="15"/>
+      <c r="X59" s="15"/>
+      <c r="Y59" s="15"/>
+      <c r="Z59" s="15"/>
+      <c r="AA59" s="15"/>
+      <c r="AB59" s="15"/>
+      <c r="AC59" s="15"/>
+      <c r="AD59" s="15"/>
+      <c r="AE59" s="15"/>
+      <c r="AF59" s="15"/>
+      <c r="AG59" s="15"/>
+      <c r="AH59" s="15"/>
+      <c r="AI59" s="15"/>
+      <c r="AJ59" s="15"/>
+      <c r="AK59" s="15"/>
+      <c r="AL59" s="15"/>
+      <c r="AM59" s="15"/>
+      <c r="AN59" s="15"/>
+      <c r="AO59" s="15"/>
+      <c r="AP59" s="15"/>
+      <c r="AQ59" s="15"/>
+      <c r="AR59" s="15"/>
+      <c r="AS59" s="15"/>
+      <c r="AT59" s="15"/>
+      <c r="AU59" s="15"/>
+      <c r="AV59" s="15"/>
+      <c r="AW59" s="15"/>
+      <c r="AX59" s="15"/>
+      <c r="AY59" s="15"/>
+      <c r="AZ59" s="15"/>
+      <c r="BA59" s="15"/>
+      <c r="BB59" s="15"/>
+      <c r="BC59" s="15"/>
+      <c r="BD59" s="15"/>
+      <c r="BE59" s="15"/>
+      <c r="BF59" s="15"/>
+      <c r="BG59" s="15"/>
+      <c r="BH59" s="15"/>
+      <c r="BI59" s="15"/>
+      <c r="BJ59" s="15"/>
+      <c r="BK59" s="15"/>
+      <c r="BL59" s="15"/>
+      <c r="BM59" s="15"/>
+      <c r="BN59" s="15"/>
+      <c r="BO59" s="15"/>
+      <c r="BP59" s="15"/>
+      <c r="BQ59" s="15"/>
+      <c r="BR59" s="15"/>
+      <c r="BS59" s="15"/>
+      <c r="BT59" s="15"/>
+      <c r="BU59" s="15"/>
+      <c r="BV59" s="15"/>
+      <c r="BW59" s="15"/>
+      <c r="BX59" s="15"/>
+      <c r="BY59" s="16"/>
     </row>
     <row r="60" spans="1:77" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="8" t="s">
+      <c r="A60" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B60" s="8">
+      <c r="B60" s="10">
         <v>2019</v>
       </c>
-      <c r="C60" s="8"/>
-      <c r="D60" s="8">
+      <c r="C60" s="11"/>
+      <c r="D60" s="10">
         <v>2018</v>
       </c>
-      <c r="E60" s="8"/>
-      <c r="F60" s="8" t="s">
+      <c r="E60" s="11"/>
+      <c r="F60" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="G60" s="8"/>
-      <c r="H60" s="8">
+      <c r="G60" s="11"/>
+      <c r="H60" s="10">
         <v>2017</v>
       </c>
-      <c r="I60" s="8"/>
-      <c r="J60" s="8">
+      <c r="I60" s="11"/>
+      <c r="J60" s="10">
         <v>2016</v>
       </c>
-      <c r="K60" s="8"/>
-      <c r="L60" s="8">
+      <c r="K60" s="11"/>
+      <c r="L60" s="10">
         <v>2015</v>
       </c>
-      <c r="M60" s="8"/>
-      <c r="N60" s="8">
+      <c r="M60" s="11"/>
+      <c r="N60" s="10">
         <v>2014</v>
       </c>
-      <c r="O60" s="8"/>
-      <c r="P60" s="8" t="s">
+      <c r="O60" s="11"/>
+      <c r="P60" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="Q60" s="8"/>
-      <c r="R60" s="8" t="s">
+      <c r="Q60" s="11"/>
+      <c r="R60" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="S60" s="8"/>
-      <c r="T60" s="8">
+      <c r="S60" s="11"/>
+      <c r="T60" s="10">
         <v>2012</v>
       </c>
-      <c r="U60" s="8"/>
-      <c r="V60" s="8">
+      <c r="U60" s="11"/>
+      <c r="V60" s="10">
         <v>2011</v>
       </c>
-      <c r="W60" s="8"/>
-      <c r="X60" s="8" t="s">
+      <c r="W60" s="11"/>
+      <c r="X60" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="Y60" s="8"/>
-      <c r="Z60" s="8" t="s">
+      <c r="Y60" s="11"/>
+      <c r="Z60" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="AA60" s="8"/>
-      <c r="AB60" s="8">
+      <c r="AA60" s="11"/>
+      <c r="AB60" s="10">
         <v>2008</v>
       </c>
-      <c r="AC60" s="8"/>
-      <c r="AD60" s="8">
+      <c r="AC60" s="11"/>
+      <c r="AD60" s="10">
         <v>2007</v>
       </c>
-      <c r="AE60" s="8"/>
-      <c r="AF60" s="8">
+      <c r="AE60" s="11"/>
+      <c r="AF60" s="10">
         <v>2006</v>
       </c>
-      <c r="AG60" s="8"/>
-      <c r="AH60" s="8">
+      <c r="AG60" s="11"/>
+      <c r="AH60" s="10">
         <v>2005</v>
       </c>
-      <c r="AI60" s="8"/>
-      <c r="AJ60" s="8" t="s">
+      <c r="AI60" s="11"/>
+      <c r="AJ60" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AK60" s="8"/>
-      <c r="AL60" s="8">
+      <c r="AK60" s="11"/>
+      <c r="AL60" s="10">
         <v>2003</v>
       </c>
-      <c r="AM60" s="8"/>
-      <c r="AN60" s="8">
+      <c r="AM60" s="11"/>
+      <c r="AN60" s="10">
         <v>2002</v>
       </c>
-      <c r="AO60" s="8"/>
-      <c r="AP60" s="8">
+      <c r="AO60" s="11"/>
+      <c r="AP60" s="10">
         <v>2001</v>
       </c>
-      <c r="AQ60" s="8"/>
-      <c r="AR60" s="8" t="s">
+      <c r="AQ60" s="11"/>
+      <c r="AR60" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="AS60" s="8"/>
-      <c r="AT60" s="8" t="s">
+      <c r="AS60" s="11"/>
+      <c r="AT60" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="AU60" s="8"/>
-      <c r="AV60" s="8">
+      <c r="AU60" s="11"/>
+      <c r="AV60" s="10">
         <v>1998</v>
       </c>
-      <c r="AW60" s="8"/>
-      <c r="AX60" s="8">
+      <c r="AW60" s="11"/>
+      <c r="AX60" s="10">
         <v>1997</v>
       </c>
-      <c r="AY60" s="8"/>
-      <c r="AZ60" s="8">
+      <c r="AY60" s="11"/>
+      <c r="AZ60" s="10">
         <v>1996</v>
       </c>
-      <c r="BA60" s="8"/>
-      <c r="BB60" s="8" t="s">
+      <c r="BA60" s="11"/>
+      <c r="BB60" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="BC60" s="8"/>
-      <c r="BD60" s="8" t="s">
+      <c r="BC60" s="11"/>
+      <c r="BD60" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="BE60" s="8"/>
-      <c r="BF60" s="8" t="s">
+      <c r="BE60" s="11"/>
+      <c r="BF60" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="BG60" s="8"/>
-      <c r="BH60" s="8" t="s">
+      <c r="BG60" s="11"/>
+      <c r="BH60" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="BI60" s="8"/>
-      <c r="BJ60" s="8">
+      <c r="BI60" s="11"/>
+      <c r="BJ60" s="10">
         <v>1991</v>
       </c>
-      <c r="BK60" s="8"/>
-      <c r="BL60" s="8">
+      <c r="BK60" s="11"/>
+      <c r="BL60" s="10">
         <v>1990</v>
       </c>
-      <c r="BM60" s="8"/>
-      <c r="BN60" s="8">
+      <c r="BM60" s="11"/>
+      <c r="BN60" s="10">
         <v>1989</v>
       </c>
-      <c r="BO60" s="8"/>
-      <c r="BP60" s="8">
+      <c r="BO60" s="11"/>
+      <c r="BP60" s="10">
         <v>1988</v>
       </c>
-      <c r="BQ60" s="8"/>
-      <c r="BR60" s="8" t="s">
+      <c r="BQ60" s="11"/>
+      <c r="BR60" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="BS60" s="8"/>
-      <c r="BT60" s="8">
+      <c r="BS60" s="11"/>
+      <c r="BT60" s="10">
         <v>1986</v>
       </c>
-      <c r="BU60" s="8"/>
-      <c r="BV60" s="8" t="s">
+      <c r="BU60" s="11"/>
+      <c r="BV60" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="BW60" s="8"/>
-      <c r="BX60" s="8" t="s">
+      <c r="BW60" s="11"/>
+      <c r="BX60" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="BY60" s="8"/>
+      <c r="BY60" s="11"/>
     </row>
     <row r="61" spans="1:77" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="8"/>
+      <c r="A61" s="13"/>
       <c r="B61" s="1" t="s">
         <v>4</v>
       </c>
@@ -26234,169 +26344,238 @@
       </c>
     </row>
     <row r="114" spans="1:77" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A114" s="9" t="s">
+      <c r="A114" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="B114" s="9"/>
-      <c r="C114" s="9"/>
-      <c r="D114" s="9"/>
-      <c r="E114" s="9"/>
-      <c r="F114" s="9"/>
-      <c r="G114" s="9"/>
-      <c r="H114" s="9"/>
-      <c r="I114" s="9"/>
-      <c r="J114" s="9"/>
-      <c r="K114" s="9"/>
-      <c r="L114" s="9"/>
-      <c r="M114" s="9"/>
-      <c r="N114" s="9"/>
-      <c r="O114" s="9"/>
-      <c r="P114" s="9"/>
-      <c r="Q114" s="9"/>
-      <c r="R114" s="9"/>
-      <c r="S114" s="9"/>
-      <c r="T114" s="9"/>
-      <c r="U114" s="9"/>
-      <c r="V114" s="9"/>
-      <c r="W114" s="9"/>
-      <c r="X114" s="9"/>
-      <c r="Y114" s="9"/>
-      <c r="Z114" s="9"/>
-      <c r="AA114" s="9"/>
-      <c r="AB114" s="9"/>
-      <c r="AC114" s="9"/>
-      <c r="AD114" s="9"/>
-      <c r="AE114" s="9"/>
-      <c r="AF114" s="9"/>
-      <c r="AG114" s="9"/>
-      <c r="AH114" s="9"/>
-      <c r="AI114" s="9"/>
-      <c r="AJ114" s="9"/>
-      <c r="AK114" s="9"/>
-      <c r="AL114" s="9"/>
-      <c r="AM114" s="9"/>
-      <c r="AN114" s="9"/>
-      <c r="AO114" s="9"/>
-      <c r="AP114" s="9"/>
-      <c r="AQ114" s="9"/>
-      <c r="AR114" s="9"/>
-      <c r="AS114" s="9"/>
-      <c r="AT114" s="9"/>
-      <c r="AU114" s="9"/>
-      <c r="AV114" s="9"/>
-      <c r="AW114" s="9"/>
-      <c r="AX114" s="9"/>
-      <c r="AY114" s="9"/>
-      <c r="AZ114" s="9"/>
-      <c r="BA114" s="9"/>
-      <c r="BB114" s="9"/>
-      <c r="BC114" s="9"/>
-      <c r="BD114" s="9"/>
-      <c r="BE114" s="9"/>
-      <c r="BF114" s="9"/>
-      <c r="BG114" s="9"/>
-      <c r="BH114" s="9"/>
-      <c r="BI114" s="9"/>
-      <c r="BJ114" s="9"/>
-      <c r="BK114" s="9"/>
-      <c r="BL114" s="9"/>
-      <c r="BM114" s="9"/>
-      <c r="BN114" s="9"/>
-      <c r="BO114" s="9"/>
-      <c r="BP114" s="9"/>
-      <c r="BQ114" s="9"/>
-      <c r="BR114" s="9"/>
-      <c r="BS114" s="9"/>
-      <c r="BT114" s="9"/>
-      <c r="BU114" s="9"/>
-      <c r="BV114" s="9"/>
-      <c r="BW114" s="9"/>
-      <c r="BX114" s="9"/>
-      <c r="BY114" s="9"/>
+      <c r="B114" s="5"/>
+      <c r="C114" s="5"/>
+      <c r="D114" s="5"/>
+      <c r="E114" s="5"/>
+      <c r="F114" s="5"/>
+      <c r="G114" s="5"/>
+      <c r="H114" s="5"/>
+      <c r="I114" s="5"/>
+      <c r="J114" s="5"/>
+      <c r="K114" s="5"/>
+      <c r="L114" s="5"/>
+      <c r="M114" s="5"/>
+      <c r="N114" s="5"/>
+      <c r="O114" s="5"/>
+      <c r="P114" s="5"/>
+      <c r="Q114" s="5"/>
+      <c r="R114" s="5"/>
+      <c r="S114" s="5"/>
+      <c r="T114" s="5"/>
+      <c r="U114" s="5"/>
+      <c r="V114" s="5"/>
+      <c r="W114" s="5"/>
+      <c r="X114" s="5"/>
+      <c r="Y114" s="5"/>
+      <c r="Z114" s="5"/>
+      <c r="AA114" s="5"/>
+      <c r="AB114" s="5"/>
+      <c r="AC114" s="5"/>
+      <c r="AD114" s="5"/>
+      <c r="AE114" s="5"/>
+      <c r="AF114" s="5"/>
+      <c r="AG114" s="5"/>
+      <c r="AH114" s="5"/>
+      <c r="AI114" s="5"/>
+      <c r="AJ114" s="5"/>
+      <c r="AK114" s="5"/>
+      <c r="AL114" s="5"/>
+      <c r="AM114" s="5"/>
+      <c r="AN114" s="5"/>
+      <c r="AO114" s="5"/>
+      <c r="AP114" s="5"/>
+      <c r="AQ114" s="5"/>
+      <c r="AR114" s="5"/>
+      <c r="AS114" s="5"/>
+      <c r="AT114" s="5"/>
+      <c r="AU114" s="5"/>
+      <c r="AV114" s="5"/>
+      <c r="AW114" s="5"/>
+      <c r="AX114" s="5"/>
+      <c r="AY114" s="5"/>
+      <c r="AZ114" s="5"/>
+      <c r="BA114" s="5"/>
+      <c r="BB114" s="5"/>
+      <c r="BC114" s="5"/>
+      <c r="BD114" s="5"/>
+      <c r="BE114" s="5"/>
+      <c r="BF114" s="5"/>
+      <c r="BG114" s="5"/>
+      <c r="BH114" s="5"/>
+      <c r="BI114" s="5"/>
+      <c r="BJ114" s="5"/>
+      <c r="BK114" s="5"/>
+      <c r="BL114" s="5"/>
+      <c r="BM114" s="5"/>
+      <c r="BN114" s="5"/>
+      <c r="BO114" s="5"/>
+      <c r="BP114" s="5"/>
+      <c r="BQ114" s="5"/>
+      <c r="BR114" s="5"/>
+      <c r="BS114" s="5"/>
+      <c r="BT114" s="5"/>
+      <c r="BU114" s="5"/>
+      <c r="BV114" s="5"/>
+      <c r="BW114" s="5"/>
+      <c r="BX114" s="5"/>
+      <c r="BY114" s="5"/>
     </row>
     <row r="115" spans="1:77" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A115" s="9" t="s">
+      <c r="A115" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="B115" s="9"/>
-      <c r="C115" s="9"/>
-      <c r="D115" s="9"/>
-      <c r="E115" s="9"/>
-      <c r="F115" s="9"/>
-      <c r="G115" s="9"/>
-      <c r="H115" s="9"/>
-      <c r="I115" s="9"/>
-      <c r="J115" s="9"/>
-      <c r="K115" s="9"/>
-      <c r="L115" s="9"/>
-      <c r="M115" s="9"/>
-      <c r="N115" s="9"/>
-      <c r="O115" s="9"/>
-      <c r="P115" s="9"/>
-      <c r="Q115" s="9"/>
-      <c r="R115" s="9"/>
-      <c r="S115" s="9"/>
-      <c r="T115" s="9"/>
-      <c r="U115" s="9"/>
-      <c r="V115" s="9"/>
-      <c r="W115" s="9"/>
-      <c r="X115" s="9"/>
-      <c r="Y115" s="9"/>
-      <c r="Z115" s="9"/>
-      <c r="AA115" s="9"/>
-      <c r="AB115" s="9"/>
-      <c r="AC115" s="9"/>
-      <c r="AD115" s="9"/>
-      <c r="AE115" s="9"/>
-      <c r="AF115" s="9"/>
-      <c r="AG115" s="9"/>
-      <c r="AH115" s="9"/>
-      <c r="AI115" s="9"/>
-      <c r="AJ115" s="9"/>
-      <c r="AK115" s="9"/>
-      <c r="AL115" s="9"/>
-      <c r="AM115" s="9"/>
-      <c r="AN115" s="9"/>
-      <c r="AO115" s="9"/>
-      <c r="AP115" s="9"/>
-      <c r="AQ115" s="9"/>
-      <c r="AR115" s="9"/>
-      <c r="AS115" s="9"/>
-      <c r="AT115" s="9"/>
-      <c r="AU115" s="9"/>
-      <c r="AV115" s="9"/>
-      <c r="AW115" s="9"/>
-      <c r="AX115" s="9"/>
-      <c r="AY115" s="9"/>
-      <c r="AZ115" s="9"/>
-      <c r="BA115" s="9"/>
-      <c r="BB115" s="9"/>
-      <c r="BC115" s="9"/>
-      <c r="BD115" s="9"/>
-      <c r="BE115" s="9"/>
-      <c r="BF115" s="9"/>
-      <c r="BG115" s="9"/>
-      <c r="BH115" s="9"/>
-      <c r="BI115" s="9"/>
-      <c r="BJ115" s="9"/>
-      <c r="BK115" s="9"/>
-      <c r="BL115" s="9"/>
-      <c r="BM115" s="9"/>
-      <c r="BN115" s="9"/>
-      <c r="BO115" s="9"/>
-      <c r="BP115" s="9"/>
-      <c r="BQ115" s="9"/>
-      <c r="BR115" s="9"/>
-      <c r="BS115" s="9"/>
-      <c r="BT115" s="9"/>
-      <c r="BU115" s="9"/>
-      <c r="BV115" s="9"/>
-      <c r="BW115" s="9"/>
-      <c r="BX115" s="9"/>
-      <c r="BY115" s="9"/>
+      <c r="B115" s="5"/>
+      <c r="C115" s="5"/>
+      <c r="D115" s="5"/>
+      <c r="E115" s="5"/>
+      <c r="F115" s="5"/>
+      <c r="G115" s="5"/>
+      <c r="H115" s="5"/>
+      <c r="I115" s="5"/>
+      <c r="J115" s="5"/>
+      <c r="K115" s="5"/>
+      <c r="L115" s="5"/>
+      <c r="M115" s="5"/>
+      <c r="N115" s="5"/>
+      <c r="O115" s="5"/>
+      <c r="P115" s="5"/>
+      <c r="Q115" s="5"/>
+      <c r="R115" s="5"/>
+      <c r="S115" s="5"/>
+      <c r="T115" s="5"/>
+      <c r="U115" s="5"/>
+      <c r="V115" s="5"/>
+      <c r="W115" s="5"/>
+      <c r="X115" s="5"/>
+      <c r="Y115" s="5"/>
+      <c r="Z115" s="5"/>
+      <c r="AA115" s="5"/>
+      <c r="AB115" s="5"/>
+      <c r="AC115" s="5"/>
+      <c r="AD115" s="5"/>
+      <c r="AE115" s="5"/>
+      <c r="AF115" s="5"/>
+      <c r="AG115" s="5"/>
+      <c r="AH115" s="5"/>
+      <c r="AI115" s="5"/>
+      <c r="AJ115" s="5"/>
+      <c r="AK115" s="5"/>
+      <c r="AL115" s="5"/>
+      <c r="AM115" s="5"/>
+      <c r="AN115" s="5"/>
+      <c r="AO115" s="5"/>
+      <c r="AP115" s="5"/>
+      <c r="AQ115" s="5"/>
+      <c r="AR115" s="5"/>
+      <c r="AS115" s="5"/>
+      <c r="AT115" s="5"/>
+      <c r="AU115" s="5"/>
+      <c r="AV115" s="5"/>
+      <c r="AW115" s="5"/>
+      <c r="AX115" s="5"/>
+      <c r="AY115" s="5"/>
+      <c r="AZ115" s="5"/>
+      <c r="BA115" s="5"/>
+      <c r="BB115" s="5"/>
+      <c r="BC115" s="5"/>
+      <c r="BD115" s="5"/>
+      <c r="BE115" s="5"/>
+      <c r="BF115" s="5"/>
+      <c r="BG115" s="5"/>
+      <c r="BH115" s="5"/>
+      <c r="BI115" s="5"/>
+      <c r="BJ115" s="5"/>
+      <c r="BK115" s="5"/>
+      <c r="BL115" s="5"/>
+      <c r="BM115" s="5"/>
+      <c r="BN115" s="5"/>
+      <c r="BO115" s="5"/>
+      <c r="BP115" s="5"/>
+      <c r="BQ115" s="5"/>
+      <c r="BR115" s="5"/>
+      <c r="BS115" s="5"/>
+      <c r="BT115" s="5"/>
+      <c r="BU115" s="5"/>
+      <c r="BV115" s="5"/>
+      <c r="BW115" s="5"/>
+      <c r="BX115" s="5"/>
+      <c r="BY115" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="85">
+    <mergeCell ref="D60:E60"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="A60:A61"/>
+    <mergeCell ref="A59:BY59"/>
+    <mergeCell ref="N60:O60"/>
+    <mergeCell ref="L60:M60"/>
+    <mergeCell ref="J60:K60"/>
+    <mergeCell ref="H60:I60"/>
+    <mergeCell ref="F60:G60"/>
+    <mergeCell ref="X60:Y60"/>
+    <mergeCell ref="V60:W60"/>
+    <mergeCell ref="T60:U60"/>
+    <mergeCell ref="R60:S60"/>
+    <mergeCell ref="P60:Q60"/>
+    <mergeCell ref="A1:BY1"/>
+    <mergeCell ref="A2:BY2"/>
+    <mergeCell ref="A3:BY3"/>
+    <mergeCell ref="A4:BY4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="L5:M5"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="V5:W5"/>
+    <mergeCell ref="X5:Y5"/>
+    <mergeCell ref="Z5:AA5"/>
+    <mergeCell ref="AB5:AC5"/>
+    <mergeCell ref="AD5:AE5"/>
+    <mergeCell ref="AF5:AG5"/>
+    <mergeCell ref="AH5:AI5"/>
+    <mergeCell ref="AJ5:AK5"/>
+    <mergeCell ref="AL5:AM5"/>
+    <mergeCell ref="AN5:AO5"/>
+    <mergeCell ref="AP5:AQ5"/>
+    <mergeCell ref="AR5:AS5"/>
+    <mergeCell ref="AT5:AU5"/>
+    <mergeCell ref="AV5:AW5"/>
+    <mergeCell ref="AX5:AY5"/>
+    <mergeCell ref="AZ5:BA5"/>
+    <mergeCell ref="BB5:BC5"/>
+    <mergeCell ref="BD5:BE5"/>
+    <mergeCell ref="BF5:BG5"/>
+    <mergeCell ref="BH5:BI5"/>
+    <mergeCell ref="BJ5:BK5"/>
+    <mergeCell ref="BL5:BM5"/>
+    <mergeCell ref="BN5:BO5"/>
+    <mergeCell ref="BP5:BQ5"/>
+    <mergeCell ref="BR5:BS5"/>
+    <mergeCell ref="BT5:BU5"/>
+    <mergeCell ref="BV5:BW5"/>
+    <mergeCell ref="BX5:BY5"/>
+    <mergeCell ref="Z60:AA60"/>
+    <mergeCell ref="AB60:AC60"/>
+    <mergeCell ref="AD60:AE60"/>
+    <mergeCell ref="AF60:AG60"/>
+    <mergeCell ref="AH60:AI60"/>
+    <mergeCell ref="AZ60:BA60"/>
+    <mergeCell ref="BB60:BC60"/>
+    <mergeCell ref="AJ60:AK60"/>
+    <mergeCell ref="AL60:AM60"/>
+    <mergeCell ref="AN60:AO60"/>
+    <mergeCell ref="AP60:AQ60"/>
+    <mergeCell ref="AR60:AS60"/>
     <mergeCell ref="BX60:BY60"/>
     <mergeCell ref="A114:BY114"/>
     <mergeCell ref="A115:BY115"/>
@@ -26413,75 +26592,6 @@
     <mergeCell ref="AT60:AU60"/>
     <mergeCell ref="AV60:AW60"/>
     <mergeCell ref="AX60:AY60"/>
-    <mergeCell ref="AZ60:BA60"/>
-    <mergeCell ref="BB60:BC60"/>
-    <mergeCell ref="AJ60:AK60"/>
-    <mergeCell ref="AL60:AM60"/>
-    <mergeCell ref="AN60:AO60"/>
-    <mergeCell ref="AP60:AQ60"/>
-    <mergeCell ref="AR60:AS60"/>
-    <mergeCell ref="Z60:AA60"/>
-    <mergeCell ref="AB60:AC60"/>
-    <mergeCell ref="AD60:AE60"/>
-    <mergeCell ref="AF60:AG60"/>
-    <mergeCell ref="AH60:AI60"/>
-    <mergeCell ref="BV5:BW5"/>
-    <mergeCell ref="BX5:BY5"/>
-    <mergeCell ref="A59:BY59"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="D60:E60"/>
-    <mergeCell ref="F60:G60"/>
-    <mergeCell ref="H60:I60"/>
-    <mergeCell ref="J60:K60"/>
-    <mergeCell ref="L60:M60"/>
-    <mergeCell ref="N60:O60"/>
-    <mergeCell ref="P60:Q60"/>
-    <mergeCell ref="R60:S60"/>
-    <mergeCell ref="T60:U60"/>
-    <mergeCell ref="V60:W60"/>
-    <mergeCell ref="X60:Y60"/>
-    <mergeCell ref="BL5:BM5"/>
-    <mergeCell ref="BN5:BO5"/>
-    <mergeCell ref="BP5:BQ5"/>
-    <mergeCell ref="BR5:BS5"/>
-    <mergeCell ref="BT5:BU5"/>
-    <mergeCell ref="BB5:BC5"/>
-    <mergeCell ref="BD5:BE5"/>
-    <mergeCell ref="BF5:BG5"/>
-    <mergeCell ref="BH5:BI5"/>
-    <mergeCell ref="BJ5:BK5"/>
-    <mergeCell ref="AR5:AS5"/>
-    <mergeCell ref="AT5:AU5"/>
-    <mergeCell ref="AV5:AW5"/>
-    <mergeCell ref="AX5:AY5"/>
-    <mergeCell ref="AZ5:BA5"/>
-    <mergeCell ref="AH5:AI5"/>
-    <mergeCell ref="AJ5:AK5"/>
-    <mergeCell ref="AL5:AM5"/>
-    <mergeCell ref="AN5:AO5"/>
-    <mergeCell ref="AP5:AQ5"/>
-    <mergeCell ref="X5:Y5"/>
-    <mergeCell ref="Z5:AA5"/>
-    <mergeCell ref="AB5:AC5"/>
-    <mergeCell ref="AD5:AE5"/>
-    <mergeCell ref="AF5:AG5"/>
-    <mergeCell ref="A1:BY1"/>
-    <mergeCell ref="A2:BY2"/>
-    <mergeCell ref="A3:BY3"/>
-    <mergeCell ref="A4:BY4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="L5:M5"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="V5:W5"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A114" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>